<commit_message>
update data and plots for bmi
</commit_message>
<xml_diff>
--- a/data_raw/VN_BMI_2016-2018_taxa_data.xlsx
+++ b/data_raw/VN_BMI_2016-2018_taxa_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rapeek/Documents/github/van_norden_aquabio/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC3F8B3-D467-D447-B978-EEEF1363ACD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC58E206-9150-3D40-93B1-C5368AD16505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39940" yWindow="720" windowWidth="35200" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data_raw" sheetId="1" r:id="rId1"/>
     <sheet name="data_family_safit" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -58,8 +58,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="333">
   <si>
     <t>Stream</t>
   </si>
@@ -1010,13 +1032,61 @@
   </si>
   <si>
     <t>Taxon present, but without count included on data sheet</t>
+  </si>
+  <si>
+    <t>SY16</t>
+  </si>
+  <si>
+    <t>CC18</t>
+  </si>
+  <si>
+    <t>SY18</t>
+  </si>
+  <si>
+    <t>CC17</t>
+  </si>
+  <si>
+    <t>SY17</t>
+  </si>
+  <si>
+    <t>PRIMARY METRICS:</t>
+  </si>
+  <si>
+    <t>Taxa Richness:</t>
+  </si>
+  <si>
+    <t>EPT Richness:</t>
+  </si>
+  <si>
+    <t>Sensitive EPT:</t>
+  </si>
+  <si>
+    <t>% Dominant Taxon:</t>
+  </si>
+  <si>
+    <t>Tolerance Value:</t>
+  </si>
+  <si>
+    <t>Shannon's D.I.:</t>
+  </si>
+  <si>
+    <t>Percent of sample subsampled:</t>
+  </si>
+  <si>
+    <t>Estimated Relative Abundance:</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Metric</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1076,8 +1146,23 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1093,6 +1178,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1148,7 +1239,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1188,6 +1279,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1197,12 +1299,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
@@ -1556,10 +1652,10 @@
   <dimension ref="A1:AD405"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="11" ySplit="7" topLeftCell="L216" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="7" topLeftCell="L202" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D226" sqref="D226"/>
+      <selection pane="bottomRight" activeCell="I225" sqref="I225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5011,8 +5107,8 @@
       <c r="W302" s="14"/>
       <c r="X302" s="14"/>
       <c r="Y302" s="16"/>
-      <c r="Z302" s="31"/>
-      <c r="AA302" s="32"/>
+      <c r="Z302" s="40"/>
+      <c r="AA302" s="41"/>
       <c r="AB302" s="14"/>
       <c r="AC302" s="16"/>
       <c r="AD302" s="14"/>
@@ -5046,8 +5142,8 @@
       <c r="T303" s="17"/>
       <c r="U303" s="17"/>
       <c r="V303" s="17"/>
-      <c r="Z303" s="31"/>
-      <c r="AA303" s="33"/>
+      <c r="Z303" s="40"/>
+      <c r="AA303" s="42"/>
     </row>
     <row r="304" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="L304" s="22" t="s">
@@ -5078,8 +5174,8 @@
       <c r="T304" s="17"/>
       <c r="U304" s="17"/>
       <c r="V304" s="17"/>
-      <c r="Z304" s="31"/>
-      <c r="AA304" s="33"/>
+      <c r="Z304" s="40"/>
+      <c r="AA304" s="42"/>
     </row>
     <row r="305" spans="4:22" ht="42" x14ac:dyDescent="0.15">
       <c r="L305" s="22" t="s">
@@ -5623,11 +5719,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47403C2-E259-874D-900A-FA10995D49A5}">
-  <dimension ref="A1:V121"/>
+  <dimension ref="A1:W120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="7" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5636,49 +5732,49 @@
     <col min="2" max="2" width="11" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="16.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="13.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.83203125" style="13"/>
+    <col min="5" max="5" width="15" style="2" customWidth="1"/>
+    <col min="6" max="8" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="16.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6"/>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="E2" s="6"/>
       <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
@@ -5691,113 +5787,154 @@
       <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="J2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-    </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E3" s="6"/>
+      <c r="F3" s="24">
+        <v>42651</v>
+      </c>
+      <c r="G3" s="24">
+        <v>43370</v>
+      </c>
+      <c r="H3" s="24">
+        <v>43370</v>
+      </c>
+      <c r="I3" s="24">
+        <v>42989</v>
+      </c>
+      <c r="J3" s="24">
+        <v>42989</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="24">
-        <v>42651</v>
-      </c>
-      <c r="F4" s="24">
-        <v>43370</v>
-      </c>
-      <c r="G4" s="24">
-        <v>43370</v>
-      </c>
-      <c r="H4" s="24">
-        <v>42989</v>
-      </c>
-      <c r="I4" s="24">
-        <v>42989</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="5" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="25"/>
-    </row>
-    <row r="6" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
+      <c r="J4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
+    <row r="6" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+        <v>42</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="13">
+        <v>2</v>
+      </c>
+      <c r="I8" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -5808,16 +5945,16 @@
         <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
       </c>
       <c r="F9" s="13">
-        <v>2</v>
-      </c>
-      <c r="H9" s="13">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -5825,16 +5962,28 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+        <v>69</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6</v>
+      </c>
+      <c r="F10" s="13">
+        <v>4</v>
+      </c>
+      <c r="G10" s="13">
+        <v>14</v>
+      </c>
+      <c r="I10" s="13">
+        <v>6</v>
+      </c>
+      <c r="J10" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -5845,22 +5994,28 @@
         <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="13">
-        <v>4</v>
+        <v>75</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6</v>
       </c>
       <c r="F11" s="13">
-        <v>14</v>
+        <v>388</v>
+      </c>
+      <c r="G11" s="13">
+        <v>998</v>
       </c>
       <c r="H11" s="13">
-        <v>6</v>
+        <v>420</v>
       </c>
       <c r="I11" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+        <v>229</v>
+      </c>
+      <c r="J11" s="13">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -5871,25 +6026,19 @@
         <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="13">
-        <v>388</v>
-      </c>
-      <c r="F12" s="13">
-        <v>998</v>
-      </c>
-      <c r="G12" s="13">
-        <v>420</v>
-      </c>
-      <c r="H12" s="13">
-        <v>229</v>
+        <v>76</v>
+      </c>
+      <c r="E12" s="2">
+        <v>8</v>
       </c>
       <c r="I12" s="13">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+      <c r="J12" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -5900,16 +6049,16 @@
         <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="13">
+        <v>80</v>
+      </c>
+      <c r="E13" s="2">
+        <v>10</v>
+      </c>
+      <c r="I13" s="13">
         <v>2</v>
       </c>
-      <c r="I13" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -5920,13 +6069,22 @@
         <v>65</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+        <v>96</v>
+      </c>
+      <c r="E14" s="2">
+        <v>6</v>
+      </c>
+      <c r="F14" s="13">
+        <v>7</v>
+      </c>
+      <c r="I14" s="13">
+        <v>8</v>
+      </c>
+      <c r="J14" s="13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -5937,19 +6095,22 @@
         <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="13">
-        <v>7</v>
-      </c>
-      <c r="H15" s="13">
-        <v>8</v>
+        <v>98</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1</v>
       </c>
       <c r="I15" s="13">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
@@ -5957,22 +6118,25 @@
         <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="13">
-        <v>1</v>
+        <v>147</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4</v>
       </c>
       <c r="F16" s="13">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G16" s="13">
+        <v>2</v>
       </c>
       <c r="H16" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -5985,20 +6149,23 @@
       <c r="D17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="13">
         <v>22</v>
       </c>
-      <c r="F17" s="13">
+      <c r="G17" s="13">
         <v>95</v>
       </c>
-      <c r="H17" s="13">
+      <c r="I17" s="13">
         <v>79</v>
       </c>
-      <c r="I17" s="13">
+      <c r="J17" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -6011,17 +6178,20 @@
       <c r="D18" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="13">
         <v>3</v>
       </c>
-      <c r="H18" s="13">
+      <c r="I18" s="13">
         <v>1</v>
       </c>
-      <c r="I18" s="13">
+      <c r="J18" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -6034,11 +6204,14 @@
       <c r="D19" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H19" s="13">
+      <c r="E19" s="2">
+        <v>3</v>
+      </c>
+      <c r="I19" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -6051,23 +6224,26 @@
       <c r="D20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="2">
+        <v>4</v>
+      </c>
+      <c r="F20" s="13">
         <v>29</v>
       </c>
-      <c r="F20" s="13">
+      <c r="G20" s="13">
         <v>11</v>
       </c>
-      <c r="G20" s="13">
+      <c r="H20" s="13">
         <v>13</v>
-      </c>
-      <c r="H20" s="13">
-        <v>37</v>
       </c>
       <c r="I20" s="13">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="J20" s="13">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -6075,22 +6251,28 @@
         <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" s="13">
-        <v>2</v>
+        <v>151</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
       </c>
       <c r="F21" s="13">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G21" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+      <c r="I21" s="13">
+        <v>15</v>
+      </c>
+      <c r="J21" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -6101,22 +6283,22 @@
         <v>149</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="13">
-        <v>11</v>
+        <v>155</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2</v>
       </c>
       <c r="F22" s="13">
-        <v>31</v>
-      </c>
-      <c r="H22" s="13">
         <v>15</v>
       </c>
       <c r="I22" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+      <c r="J22" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -6127,19 +6309,16 @@
         <v>149</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E23" s="13">
-        <v>15</v>
-      </c>
-      <c r="H23" s="13">
-        <v>78</v>
+        <v>161</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2</v>
       </c>
       <c r="I23" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
@@ -6150,13 +6329,16 @@
         <v>149</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H24" s="13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+        <v>168</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
+      <c r="I24" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
@@ -6164,16 +6346,28 @@
         <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H25" s="13">
+        <v>179</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25" s="13">
+        <v>5</v>
+      </c>
+      <c r="G25" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="I25" s="13">
+        <v>10</v>
+      </c>
+      <c r="J25" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -6184,22 +6378,19 @@
         <v>176</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E26" s="13">
+        <v>199</v>
+      </c>
+      <c r="E26" s="2">
         <v>5</v>
       </c>
-      <c r="F26" s="13">
+      <c r="I26" s="13">
+        <v>3</v>
+      </c>
+      <c r="J26" s="13">
         <v>1</v>
       </c>
-      <c r="H26" s="13">
-        <v>10</v>
-      </c>
-      <c r="I26" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
@@ -6210,318 +6401,570 @@
         <v>176</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H27" s="13">
+        <v>206</v>
+      </c>
+      <c r="E27" s="2">
+        <v>4</v>
+      </c>
+      <c r="F27" s="13">
         <v>3</v>
+      </c>
+      <c r="G27" s="13">
+        <v>1</v>
       </c>
       <c r="I27" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>176</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E28" s="13">
-        <v>3</v>
+        <v>235</v>
+      </c>
+      <c r="E28" s="2">
+        <v>8</v>
       </c>
       <c r="F28" s="13">
         <v>1</v>
       </c>
+      <c r="G28" s="13">
+        <v>67</v>
+      </c>
       <c r="H28" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+      <c r="J28" s="13">
+        <v>6</v>
+      </c>
+      <c r="S28" s="31"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="E29" s="13">
-        <v>1</v>
+        <v>236</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E29" s="2">
+        <v>8</v>
       </c>
       <c r="F29" s="13">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="G29" s="13">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="H29" s="13">
+        <v>87</v>
       </c>
       <c r="I29" s="13">
-        <v>6</v>
-      </c>
-      <c r="R29" s="34"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+      <c r="J29" s="13">
+        <v>70</v>
+      </c>
+      <c r="S29" s="31"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E30" s="13">
-        <v>41</v>
+        <v>238</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E30" s="2">
+        <v>8</v>
       </c>
       <c r="F30" s="13">
+        <v>7</v>
+      </c>
+      <c r="G30" s="13">
+        <v>5</v>
+      </c>
+      <c r="H30" s="13">
+        <v>89</v>
+      </c>
+      <c r="I30" s="13">
+        <v>2</v>
+      </c>
+      <c r="J30" s="13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E31" s="2">
+        <v>8</v>
+      </c>
+      <c r="F31" s="13">
         <v>30</v>
       </c>
-      <c r="G30" s="13">
-        <v>87</v>
-      </c>
-      <c r="H30" s="13">
+      <c r="G31" s="13">
+        <v>31</v>
+      </c>
+      <c r="H31" s="13">
+        <v>29</v>
+      </c>
+      <c r="I31" s="13">
+        <v>13</v>
+      </c>
+      <c r="J31" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="D32" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="E32" s="32">
         <v>5</v>
       </c>
-      <c r="I30" s="13">
-        <v>70</v>
-      </c>
-      <c r="R30" s="34"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="E31" s="13">
+      <c r="F32" s="34">
+        <v>33</v>
+      </c>
+      <c r="G32" s="34">
+        <v>47</v>
+      </c>
+      <c r="H32" s="34">
+        <v>249</v>
+      </c>
+      <c r="I32" s="34">
+        <v>99</v>
+      </c>
+      <c r="J32" s="34">
+        <v>278</v>
+      </c>
+      <c r="K32" s="34"/>
+    </row>
+    <row r="33" spans="1:23" s="2" customFormat="1" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="F33" s="26">
+        <f>SUM(F$8:F$32)</f>
+        <v>603</v>
+      </c>
+      <c r="G33" s="26">
+        <f t="shared" ref="G33:J33" si="0">SUM(G$8:G$32)</f>
+        <v>1336</v>
+      </c>
+      <c r="H33" s="26">
+        <f t="shared" si="0"/>
+        <v>915</v>
+      </c>
+      <c r="I33" s="26">
+        <f t="shared" si="0"/>
+        <v>617</v>
+      </c>
+      <c r="J33" s="26">
+        <f t="shared" si="0"/>
+        <v>741</v>
+      </c>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="41"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="14"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="E34" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="S34" s="40"/>
+      <c r="T34" s="42"/>
+    </row>
+    <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="E35" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="F35" s="36">
+        <f>COUNT(F$8:F$32)</f>
+        <v>18</v>
+      </c>
+      <c r="G35" s="36">
+        <f>COUNT(G$8:G$32)</f>
+        <v>15</v>
+      </c>
+      <c r="H35" s="36">
+        <f>COUNT(H$8:H$32)</f>
+        <v>8</v>
+      </c>
+      <c r="I35" s="36">
+        <f>COUNT(I$8:I$32)</f>
+        <v>22</v>
+      </c>
+      <c r="J35" s="36">
+        <f>COUNT(J$8:J$32)</f>
+        <v>16</v>
+      </c>
+      <c r="K35" s="36"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+    </row>
+    <row r="36" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="E36" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="F36" s="36">
+        <f>COUNT(F$17:F$27)</f>
         <v>7</v>
       </c>
-      <c r="F31" s="13">
+      <c r="G36" s="36">
+        <f t="shared" ref="G36:J36" si="1">COUNT(G$17:G$27)</f>
         <v>5</v>
       </c>
-      <c r="G31" s="13">
-        <v>89</v>
-      </c>
-      <c r="H31" s="13">
-        <v>2</v>
-      </c>
-      <c r="I31" s="13">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13">
-        <v>30</v>
-      </c>
-      <c r="F32" s="13">
-        <v>31</v>
-      </c>
-      <c r="G32" s="13">
-        <v>29</v>
-      </c>
-      <c r="H32" s="13">
-        <v>13</v>
-      </c>
-      <c r="I32" s="13">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>277</v>
-      </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37">
-        <v>33</v>
-      </c>
-      <c r="F33" s="37">
-        <v>47</v>
-      </c>
-      <c r="G33" s="37">
-        <v>249</v>
-      </c>
-      <c r="H33" s="37">
-        <v>99</v>
-      </c>
-      <c r="I33" s="37">
-        <v>278</v>
-      </c>
-      <c r="J33" s="37"/>
-    </row>
-    <row r="34" spans="1:22" s="2" customFormat="1" ht="14" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="32"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="14"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="R35" s="31"/>
-      <c r="S35" s="33"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="H36" s="36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I36" s="36">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J36" s="36">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="K36" s="36"/>
+    </row>
+    <row r="37" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="E37" s="37" t="s">
+        <v>325</v>
+      </c>
+      <c r="F37" s="38">
+        <f>SUMIF($E$17:$E$27,"&lt;4",F$17:F$27)/F$33*100</f>
+        <v>9.2868988391376437</v>
+      </c>
+      <c r="G37" s="38">
+        <f t="shared" ref="G37:J37" si="2">SUMIF($E$17:$E$27,"&lt;4",G$17:G$27)/G$33*100</f>
+        <v>9.5059880239520957</v>
+      </c>
+      <c r="H37" s="38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="38">
+        <f t="shared" si="2"/>
+        <v>31.604538087520261</v>
+      </c>
+      <c r="J37" s="38">
+        <f t="shared" si="2"/>
+        <v>2.9689608636977058</v>
+      </c>
+      <c r="K37" s="38"/>
+    </row>
+    <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="E38" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="F38" s="38">
+        <f>MAX(F$8:F$32)/F$33*100</f>
+        <v>64.344941956882252</v>
+      </c>
+      <c r="G38" s="38">
+        <f t="shared" ref="G38:J38" si="3">MAX(G$8:G$32)/G$33*100</f>
+        <v>74.700598802395206</v>
+      </c>
+      <c r="H38" s="38">
+        <f t="shared" si="3"/>
+        <v>45.901639344262293</v>
+      </c>
+      <c r="I38" s="38">
+        <f t="shared" si="3"/>
+        <v>37.115072933549428</v>
+      </c>
+      <c r="J38" s="38">
+        <f t="shared" si="3"/>
+        <v>37.51686909581646</v>
+      </c>
+      <c r="K38" s="38"/>
+    </row>
+    <row r="39" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="E39" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="F39" s="36" cm="1">
+        <f t="array" ref="F39">SUMPRODUCT($E$8:$E$32/F$33,F$8:F$32)</f>
+        <v>5.7064676616915433</v>
+      </c>
+      <c r="G39" s="36" cm="1">
+        <f t="array" ref="G39">SUMPRODUCT($E$8:$E$32/G$33,G$8:G$32)</f>
+        <v>5.7350299401197615</v>
+      </c>
+      <c r="H39" s="36" cm="1">
+        <f t="array" ref="H39">SUMPRODUCT($E$8:$E$32/H$33,H$8:H$32)</f>
+        <v>6.1956284153005461</v>
+      </c>
+      <c r="I39" s="36" cm="1">
+        <f t="array" ref="I39">SUMPRODUCT($E$8:$E$32/I$33,I$8:I$32)</f>
+        <v>4.474878444084279</v>
+      </c>
+      <c r="J39" s="36" cm="1">
+        <f t="array" ref="J39">SUMPRODUCT($E$8:$E$32/J$33,J$8:J$32)</f>
+        <v>5.7705802968960871</v>
+      </c>
+      <c r="K39" s="38"/>
+    </row>
+    <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="E40" s="37" t="s">
+        <v>328</v>
+      </c>
+      <c r="F40" s="36">
+        <v>1.4864740000000001</v>
+      </c>
+      <c r="G40" s="36">
+        <v>1.077437</v>
+      </c>
+      <c r="H40" s="36">
+        <v>1.448936</v>
+      </c>
+      <c r="I40" s="36">
+        <v>2.020162</v>
+      </c>
+      <c r="J40" s="38">
+        <v>1.67527</v>
+      </c>
+      <c r="K40" s="36"/>
+    </row>
+    <row r="41" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="36"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="E41" s="37" t="s">
+        <v>329</v>
+      </c>
+      <c r="F41" s="38">
+        <v>50</v>
+      </c>
+      <c r="G41" s="38">
+        <v>12.5</v>
+      </c>
+      <c r="H41" s="38">
+        <v>25</v>
+      </c>
+      <c r="I41" s="38">
+        <v>62.5</v>
+      </c>
+      <c r="J41" s="38">
+        <v>62.5</v>
+      </c>
+      <c r="K41" s="38"/>
+    </row>
+    <row r="42" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="36"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="E42" s="37" t="s">
+        <v>330</v>
+      </c>
+      <c r="F42" s="36">
+        <f>F33/F41*100</f>
+        <v>1206</v>
+      </c>
+      <c r="G42" s="36">
+        <f t="shared" ref="G42:J42" si="4">G33/G41*100</f>
+        <v>10688</v>
+      </c>
+      <c r="H42" s="36">
+        <f t="shared" si="4"/>
+        <v>3660</v>
+      </c>
+      <c r="I42" s="36">
+        <f t="shared" si="4"/>
+        <v>987.2</v>
+      </c>
+      <c r="J42" s="36">
+        <f t="shared" si="4"/>
+        <v>1185.5999999999999</v>
+      </c>
+      <c r="K42" s="39"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.15">
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" s="2"/>
-      <c r="J51" s="21"/>
       <c r="K51" s="21"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L51" s="21"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52" s="2"/>
-      <c r="J52" s="21"/>
       <c r="K52" s="21"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L52" s="21"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" s="2"/>
-      <c r="J53" s="21"/>
       <c r="K53" s="21"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L53" s="21"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54" s="2"/>
-      <c r="J54" s="21"/>
       <c r="K54" s="21"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L54" s="21"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55" s="2"/>
-      <c r="J55" s="21"/>
       <c r="K55" s="21"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L55" s="21"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A56" s="2"/>
-      <c r="J56" s="21"/>
       <c r="K56" s="21"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L56" s="21"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A57" s="2"/>
-      <c r="J57" s="21"/>
       <c r="K57" s="21"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L57" s="21"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A58" s="2"/>
-      <c r="J58" s="21"/>
       <c r="K58" s="21"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L58" s="21"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A59" s="2"/>
-      <c r="J59" s="21"/>
-      <c r="K59" s="21"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A60" s="2"/>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D67" s="13"/>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D70" s="13"/>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="E70" s="13"/>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D71" s="13"/>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D72" s="13"/>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="E71" s="13"/>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D74" s="13"/>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D75" s="13"/>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="E74" s="13"/>
+    </row>
+    <row r="76" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+    </row>
+    <row r="77" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D77" s="13"/>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D78" s="13"/>
+      <c r="E77" s="13"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" s="2"/>
@@ -6548,13 +6991,12 @@
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C97" s="2"/>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C96" s="2"/>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B107" s="2"/>
@@ -6568,35 +7010,38 @@
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="114" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D115" s="13"/>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="E115" s="13"/>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D116" s="13"/>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="E116" s="13"/>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D117" s="13"/>
-    </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="E117" s="13"/>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D118" s="13"/>
-    </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="E118" s="13"/>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D119" s="13"/>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="E119" s="13"/>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D120" s="13"/>
-    </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D121" s="13"/>
+      <c r="E120" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="R34:R35"/>
-    <mergeCell ref="S34:S35"/>
+    <mergeCell ref="S33:S34"/>
+    <mergeCell ref="T33:T34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="200"/>

</xml_diff>

<commit_message>
update data and figs for report
</commit_message>
<xml_diff>
--- a/data_raw/VN_BMI_2016-2018_taxa_data.xlsx
+++ b/data_raw/VN_BMI_2016-2018_taxa_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rapeek/Documents/github/van_norden_aquabio/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5E31D0-BD78-CC4E-BD1A-50A6E3EF82B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCDDB30-63E4-9C43-93F6-F7530517DDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_raw" sheetId="1" r:id="rId1"/>
@@ -1293,6 +1293,8 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1302,8 +1304,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
@@ -5112,8 +5112,8 @@
       <c r="W302" s="14"/>
       <c r="X302" s="14"/>
       <c r="Y302" s="16"/>
-      <c r="Z302" s="40"/>
-      <c r="AA302" s="41"/>
+      <c r="Z302" s="42"/>
+      <c r="AA302" s="43"/>
       <c r="AB302" s="14"/>
       <c r="AC302" s="16"/>
       <c r="AD302" s="14"/>
@@ -5147,8 +5147,8 @@
       <c r="T303" s="17"/>
       <c r="U303" s="17"/>
       <c r="V303" s="17"/>
-      <c r="Z303" s="40"/>
-      <c r="AA303" s="42"/>
+      <c r="Z303" s="42"/>
+      <c r="AA303" s="44"/>
     </row>
     <row r="304" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="L304" s="22" t="s">
@@ -5179,8 +5179,8 @@
       <c r="T304" s="17"/>
       <c r="U304" s="17"/>
       <c r="V304" s="17"/>
-      <c r="Z304" s="40"/>
-      <c r="AA304" s="42"/>
+      <c r="Z304" s="42"/>
+      <c r="AA304" s="44"/>
     </row>
     <row r="305" spans="4:22" ht="42" x14ac:dyDescent="0.15">
       <c r="L305" s="22" t="s">
@@ -5727,8 +5727,8 @@
   <dimension ref="A1:W120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
+      <pane ySplit="7" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6604,8 +6604,8 @@
       <c r="P33" s="14"/>
       <c r="Q33" s="14"/>
       <c r="R33" s="16"/>
-      <c r="S33" s="40"/>
-      <c r="T33" s="41"/>
+      <c r="S33" s="42"/>
+      <c r="T33" s="43"/>
       <c r="U33" s="14"/>
       <c r="V33" s="16"/>
       <c r="W33" s="14"/>
@@ -6634,8 +6634,8 @@
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
       <c r="O34" s="17"/>
-      <c r="S34" s="40"/>
-      <c r="T34" s="42"/>
+      <c r="S34" s="42"/>
+      <c r="T34" s="44"/>
     </row>
     <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="35" t="s">
@@ -6766,22 +6766,22 @@
       <c r="E39" s="37" t="s">
         <v>333</v>
       </c>
-      <c r="F39" s="43" t="s">
+      <c r="F39" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="G39" s="43" t="s">
+      <c r="G39" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H39" s="43" t="s">
+      <c r="H39" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="I39" s="43" t="s">
+      <c r="I39" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="J39" s="43" t="s">
+      <c r="J39" s="40" t="s">
         <v>277</v>
       </c>
-      <c r="K39" s="44"/>
+      <c r="K39" s="41"/>
     </row>
     <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="36"/>

</xml_diff>